<commit_message>
cambio de power y excel
</commit_message>
<xml_diff>
--- a/FixWay.xlsx
+++ b/FixWay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inacapmailcl.sharepoint.com/sites/ProyectoTitulo382/Shared Documents/General/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="411" documentId="13_ncr:1_{0D1FD115-8C63-48DD-8A48-CB0CA4151083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80E6F67C-C96A-4FFE-8F8A-799176CED57B}"/>
+  <xr:revisionPtr revIDLastSave="416" documentId="13_ncr:1_{0D1FD115-8C63-48DD-8A48-CB0CA4151083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{215A3000-AA01-49B3-9EB3-A6526006FDEC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07A88C75-C746-4A27-AF07-AAD3CE5976C5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>COSTOS POR HORA HOMBRE</t>
   </si>
@@ -100,17 +100,13 @@
   </si>
   <si>
     <t>ROI</t>
-  </si>
-  <si>
-    <t>No va en el Proyecto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;\-#,##0.00"/>
+  <numFmts count="2">
     <numFmt numFmtId="42" formatCode="_ &quot;$&quot;* #,##0_ ;_ &quot;$&quot;* \-#,##0_ ;_ &quot;$&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
@@ -245,7 +241,7 @@
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -264,7 +260,6 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -288,12 +283,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -303,7 +298,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Millares [0]" xfId="4" builtinId="6"/>
@@ -372,10 +366,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -695,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34417596-DF64-4A0D-82CC-F333B16575B7}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,168 +703,168 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="19" t="s">
+      <c r="D2" s="33"/>
+      <c r="E2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="14">
         <f>5600000/3</f>
         <v>1866666.6666666667</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="15">
         <f>(D3*100%)/B3</f>
         <v>0.19</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
         <f>B3*19%</f>
         <v>354666.66666666669</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="16">
         <f>SUM(B3,D3)</f>
         <v>2221333.3333333335</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>50</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="14">
         <f>E3/F3</f>
         <v>44426.666666666672</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="17">
         <v>9</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="16">
         <f>G3/H3</f>
         <v>4936.2962962962965</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="14">
         <f t="shared" ref="B4:B5" si="0">5600000/3</f>
         <v>1866666.6666666667</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="15">
         <f t="shared" ref="C4:C5" si="1">(D4*100%)/B4</f>
         <v>0.19</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="14">
         <f>B4*19%</f>
         <v>354666.66666666669</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="16">
         <f t="shared" ref="E4:E5" si="2">SUM(B4,D4)</f>
         <v>2221333.3333333335</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="17">
         <v>50</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="14">
         <f>E4/F4</f>
         <v>44426.666666666672</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="17">
         <v>9</v>
       </c>
-      <c r="I4" s="17">
+      <c r="I4" s="16">
         <f>G4/H4</f>
         <v>4936.2962962962965</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <f t="shared" si="0"/>
         <v>1866666.6666666667</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="15">
         <f t="shared" si="1"/>
         <v>0.19</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <f>B5*19%</f>
         <v>354666.66666666669</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="16">
         <f t="shared" si="2"/>
         <v>2221333.3333333335</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="17">
         <v>50</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="14">
         <f>E5/F5</f>
         <v>44426.666666666672</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="17">
         <v>9</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="16">
         <f>G5/H5</f>
         <v>4936.2962962962965</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="21">
         <f>SUM(B3:B5)</f>
         <v>5600000</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="22">
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="21">
         <f>SUM(E3:E5)</f>
         <v>6664000</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="24"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
@@ -913,7 +903,7 @@
       <c r="B10">
         <v>130</v>
       </c>
-      <c r="D10" s="11"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -924,7 +914,7 @@
       </c>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -942,55 +932,76 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
-      <c r="B16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
     </row>
     <row r="17" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
-      <c r="H17" s="29" t="s">
+      <c r="H17" s="27" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="12"/>
+      <c r="B18" s="11"/>
       <c r="D18" s="4"/>
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="31"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="13"/>
+      <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="37"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="32"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="30"/>
+      <c r="F21" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="32">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
-      <c r="B22" s="37"/>
-      <c r="F22" s="10"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="37"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="32"/>
-      <c r="F23" s="28"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="30"/>
+      <c r="F23" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="28">
+        <f>(15875633/7567737)*100%</f>
+        <v>2.0978045352263166</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F25" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="29">
+        <f>((15875633-7567737)/7567737)*100%</f>
+        <v>1.0978045352263166</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1008,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B548C50-DA2E-4725-A2CD-D3F217B19CFC}">
   <dimension ref="C6:D10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,30 +1029,30 @@
   </cols>
   <sheetData>
     <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="33" t="s">
-        <v>21</v>
+      <c r="D6" s="32">
+        <v>1.2</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="28">
         <f>(15875633/7567737)*100%</f>
         <v>2.0978045352263166</v>
       </c>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="29">
         <f>((15875633-7567737)/7567737)*100%</f>
         <v>1.0978045352263166</v>
       </c>
@@ -1239,15 +1250,15 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70C79143-C8FE-4AC8-8A6C-CB62D43B2D12}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="e66619f6-c031-4193-861d-2026e987347a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>